<commit_message>
Added a folder full of caption images Created an image within the player entity to display closed captioning
</commit_message>
<xml_diff>
--- a/Temple Walk Script.xlsx
+++ b/Temple Walk Script.xlsx
@@ -407,7 +407,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -459,7 +459,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,13 +769,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="36.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="44.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="30.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="129.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="27.433571428571426" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="4" width="18.862142857142857" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="4" width="25.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="20.433571428571426" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="4" width="20.14785714285714" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="4" width="21.005" customWidth="1" bestFit="1"/>
   </cols>
@@ -809,7 +809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="32.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -838,7 +838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="32.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -867,7 +867,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="32.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -896,7 +896,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="32.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -925,7 +925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="32.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -954,7 +954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="32.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
@@ -983,7 +983,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="45.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A8" s="3" t="s">
         <v>47</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="32.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A9" s="3" t="s">
         <v>55</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="45.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A10" s="3" t="s">
         <v>62</v>
       </c>

</xml_diff>